<commit_message>
unsaved work from 238
</commit_message>
<xml_diff>
--- a/0 NeetCode/238. Product of Array Except Self/Whiteboards/Solution.xlsx
+++ b/0 NeetCode/238. Product of Array Except Self/Whiteboards/Solution.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\0 template\Whiteboards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\0 NeetCode\238. Product of Array Except Self\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713DE802-9519-4608-B352-D1C1ED0E8E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054609C8-DBBA-4D78-B5CC-376EFF1A500E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
@@ -67,7 +67,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -376,7 +376,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -384,17 +384,231 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="A1"/>
+  <dimension ref="L4:X20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="4.7109375" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="4" spans="12:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L4" s="1">
+        <v>24</v>
+      </c>
+      <c r="M4" s="1">
+        <v>24</v>
+      </c>
+      <c r="N4" s="1">
+        <v>12</v>
+      </c>
+      <c r="O4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="12:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
+        <v>2</v>
+      </c>
+      <c r="N6" s="1">
+        <v>6</v>
+      </c>
+      <c r="O6" s="1">
+        <v>24</v>
+      </c>
+      <c r="R6" s="1">
+        <v>24</v>
+      </c>
+      <c r="S6" s="1">
+        <v>12</v>
+      </c>
+      <c r="T6" s="1">
+        <v>8</v>
+      </c>
+      <c r="U6" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="12:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="1">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1">
+        <v>2</v>
+      </c>
+      <c r="N8" s="1">
+        <v>3</v>
+      </c>
+      <c r="O8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="12:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S15" s="1">
+        <v>2</v>
+      </c>
+      <c r="T15" s="1">
+        <v>3</v>
+      </c>
+      <c r="U15" s="1">
+        <v>4</v>
+      </c>
+      <c r="V15" s="1">
+        <v>5</v>
+      </c>
+      <c r="W15" s="1">
+        <v>1</v>
+      </c>
+      <c r="X15" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="12:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1</v>
+      </c>
+      <c r="N16" s="1">
+        <v>3</v>
+      </c>
+      <c r="O16" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="12:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R17" s="1">
+        <f>R15</f>
+        <v>-1</v>
+      </c>
+      <c r="S17" s="1">
+        <f>S15*R17</f>
+        <v>-2</v>
+      </c>
+      <c r="T17" s="1">
+        <f t="shared" ref="T17:X17" si="0">T15*S17</f>
+        <v>-6</v>
+      </c>
+      <c r="U17" s="1">
+        <f t="shared" si="0"/>
+        <v>-24</v>
+      </c>
+      <c r="V17" s="1">
+        <f t="shared" si="0"/>
+        <v>-120</v>
+      </c>
+      <c r="W17" s="1">
+        <f t="shared" si="0"/>
+        <v>-120</v>
+      </c>
+      <c r="X17" s="1">
+        <f t="shared" si="0"/>
+        <v>-240</v>
+      </c>
+    </row>
+    <row r="18" spans="12:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L18" s="1">
+        <f t="shared" ref="L18:M18" si="1">L16*M18</f>
+        <v>-12</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="N18" s="1">
+        <f>N16*O18</f>
+        <v>12</v>
+      </c>
+      <c r="O18" s="1">
+        <f>O16</f>
+        <v>4</v>
+      </c>
+      <c r="R18" s="1">
+        <f>R15*S18</f>
+        <v>-240</v>
+      </c>
+      <c r="S18" s="1">
+        <f t="shared" ref="R18:V18" si="2">S15*T18</f>
+        <v>240</v>
+      </c>
+      <c r="T18" s="1">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="U18" s="1">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="V18" s="1">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="W18" s="1">
+        <f>W15*X18</f>
+        <v>2</v>
+      </c>
+      <c r="X18" s="1">
+        <f>X15</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="12:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L20" s="1">
+        <f>L16</f>
+        <v>-1</v>
+      </c>
+      <c r="M20" s="1">
+        <f>M16*L20</f>
+        <v>-1</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" ref="N20:O20" si="3">N16*M20</f>
+        <v>-3</v>
+      </c>
+      <c r="O20" s="1">
+        <f t="shared" si="3"/>
+        <v>-12</v>
+      </c>
+      <c r="R20" s="1">
+        <f>$R$18/R15</f>
+        <v>240</v>
+      </c>
+      <c r="S20" s="1">
+        <f t="shared" ref="S20:X20" si="4">$R$18/S15</f>
+        <v>-120</v>
+      </c>
+      <c r="T20" s="1">
+        <f t="shared" si="4"/>
+        <v>-80</v>
+      </c>
+      <c r="U20" s="1">
+        <f t="shared" si="4"/>
+        <v>-60</v>
+      </c>
+      <c r="V20" s="1">
+        <f t="shared" si="4"/>
+        <v>-48</v>
+      </c>
+      <c r="W20" s="1">
+        <f t="shared" si="4"/>
+        <v>-240</v>
+      </c>
+      <c r="X20" s="1">
+        <f t="shared" si="4"/>
+        <v>-120</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>